<commit_message>
the serial reading the analysis script.
</commit_message>
<xml_diff>
--- a/demo/config.xlsx
+++ b/demo/config.xlsx
@@ -1,50 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wenya589/Documents/GitHub/educational-backscatter-platform/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{125F744C-E8AC-0043-A4CB-0B408F628278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A79B736-52D1-3E46-846A-869C1F64650D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10360" yWindow="11740" windowWidth="28040" windowHeight="17440" xr2:uid="{0EE33369-7434-8A46-86A5-B4188E2F3CDF}"/>
+    <workbookView xWindow="0" yWindow="8380" windowWidth="30240" windowHeight="9800" xr2:uid="{0EE33369-7434-8A46-86A5-B4188E2F3CDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>center</t>
-  </si>
-  <si>
-    <t>deviation</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>baud</t>
   </si>
   <si>
-    <t>bandwidth</t>
+    <t>carrier</t>
+  </si>
+  <si>
+    <t>d_1</t>
+  </si>
+  <si>
+    <t>d_2</t>
+  </si>
+  <si>
+    <t>Center Frequency [MHz]</t>
+  </si>
+  <si>
+    <t>Baud [kBaud]</t>
+  </si>
+  <si>
+    <t>Deviation [kHz]</t>
+  </si>
+  <si>
+    <t>Filter Size [kHz]</t>
+  </si>
+  <si>
+    <t>Frequency 1 [Hz]</t>
+  </si>
+  <si>
+    <t>Frequency 2 [Hz]</t>
+  </si>
+  <si>
+    <t>Suggested Rx Configuration</t>
   </si>
 </sst>
 </file>
@@ -80,8 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,43 +410,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A189FF18-9ABD-E74C-91A8-DF53B8CE372A}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="6" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2456597222</v>
+        <v>2450000000</v>
       </c>
       <c r="B2">
-        <v>347222</v>
+        <v>20</v>
       </c>
       <c r="C2">
+        <v>18</v>
+      </c>
+      <c r="D2">
         <v>100000</v>
       </c>
-      <c r="D2">
-        <v>794444</v>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f xml:space="preserve"> 125000000/B2</f>
+        <v>6250000</v>
+      </c>
+      <c r="B7">
+        <f>125000000/C2</f>
+        <v>6944444.444444444</v>
+      </c>
+      <c r="C7" s="1">
+        <f>(A2 + (B7+A7)/2)/1000000</f>
+        <v>2456.5972222222222</v>
+      </c>
+      <c r="D7" s="1">
+        <f>D2/1000</f>
+        <v>100</v>
+      </c>
+      <c r="E7" s="1">
+        <f xml:space="preserve"> (B7-A7)/2/1000</f>
+        <v>347.222222222222</v>
+      </c>
+      <c r="F7" s="1">
+        <f>((B7-A7)+D7)/1000</f>
+        <v>694.54444444444403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change the print function and hide crc error
</commit_message>
<xml_diff>
--- a/demo/config.xlsx
+++ b/demo/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wenya589/Documents/GitHub/educational-backscatter-platform/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A79B736-52D1-3E46-846A-869C1F64650D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AE8E3D-6051-D140-BF97-2325349AE082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8380" windowWidth="30240" windowHeight="9800" xr2:uid="{0EE33369-7434-8A46-86A5-B4188E2F3CDF}"/>
+    <workbookView xWindow="-820" yWindow="10440" windowWidth="30240" windowHeight="7980" xr2:uid="{0EE33369-7434-8A46-86A5-B4188E2F3CDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -93,14 +93,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -413,7 +429,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -422,85 +438,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>2450000000</v>
       </c>
-      <c r="B2">
-        <v>20</v>
-      </c>
-      <c r="C2">
-        <v>18</v>
-      </c>
-      <c r="D2">
-        <v>100000</v>
-      </c>
+      <c r="B2" s="1">
+        <v>100</v>
+      </c>
+      <c r="C2" s="1">
+        <v>92</v>
+      </c>
+      <c r="D2" s="1">
+        <v>40000</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="1">
         <f xml:space="preserve"> 125000000/B2</f>
-        <v>6250000</v>
-      </c>
-      <c r="B7">
+        <v>1250000</v>
+      </c>
+      <c r="B7" s="1">
         <f>125000000/C2</f>
-        <v>6944444.444444444</v>
-      </c>
-      <c r="C7" s="1">
+        <v>1358695.6521739131</v>
+      </c>
+      <c r="C7" s="2">
         <f>(A2 + (B7+A7)/2)/1000000</f>
-        <v>2456.5972222222222</v>
-      </c>
-      <c r="D7" s="1">
+        <v>2451.304347826087</v>
+      </c>
+      <c r="D7" s="2">
         <f>D2/1000</f>
-        <v>100</v>
-      </c>
-      <c r="E7" s="1">
+        <v>40</v>
+      </c>
+      <c r="E7" s="2">
         <f xml:space="preserve"> (B7-A7)/2/1000</f>
-        <v>347.222222222222</v>
-      </c>
-      <c r="F7" s="1">
+        <v>54.347826086956545</v>
+      </c>
+      <c r="F7" s="2">
         <f>((B7-A7)+D7)/1000</f>
-        <v>694.54444444444403</v>
+        <v>108.73565217391308</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>$D$2/1000</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>